<commit_message>
action depens on sp not done...
</commit_message>
<xml_diff>
--- a/Document/Player Action.xlsx
+++ b/Document/Player Action.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="81">
   <si>
     <t>Player</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Earthquake</t>
   </si>
   <si>
-    <t>Wind</t>
-  </si>
-  <si>
     <t>Strom</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>Agni (Calm)</t>
   </si>
   <si>
-    <t>Attack Boost all</t>
-  </si>
-  <si>
     <t>Sp Cost</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>Random 3 Enemy</t>
   </si>
   <si>
-    <t>one Row of enemy</t>
-  </si>
-  <si>
     <t>Front collum of enemy</t>
   </si>
   <si>
@@ -257,9 +248,6 @@
     <t>Attack *.75 Variation 20%</t>
   </si>
   <si>
-    <t>Attack *1 Variation 20%</t>
-  </si>
-  <si>
     <t>Attack *1.25 Variation 20%</t>
   </si>
   <si>
@@ -267,6 +255,18 @@
   </si>
   <si>
     <t>AGNI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>Attack *1  Variation 20%</t>
+  </si>
+  <si>
+    <t>on row of enemy</t>
   </si>
 </sst>
 </file>
@@ -704,7 +704,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,141 +726,141 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" s="5">
         <v>0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H2" s="5">
         <v>0</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5">
-        <v>0</v>
+      <c r="D3" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H3" s="5">
         <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H4" s="5">
         <v>50</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="D5" s="11">
         <v>0</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H5" s="11">
         <v>0</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="11" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -871,22 +871,22 @@
         <v>0</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H6" s="11">
         <v>50</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -894,16 +894,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="11">
         <v>20</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -911,45 +911,45 @@
         <v>5</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="11">
         <v>50</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="16" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>36</v>
-      </c>
       <c r="D9" s="16">
         <v>0</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H9" s="16">
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="16" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -960,71 +960,71 @@
         <v>0</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H10" s="16">
         <v>20</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F11" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H11" s="16">
         <v>50</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="14" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="D12" s="14">
         <v>0</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H12" s="14">
         <v>0</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="14" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,19 @@
         <v>0</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="14">
+        <v>30</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1043,59 +1055,59 @@
         <v>8</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="14">
         <v>10</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="14">
         <v>40</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="9" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" s="9">
         <v>0</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H16" s="9">
         <v>0</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="9" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1106,62 +1118,77 @@
         <v>0</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H17" s="9">
         <v>30</v>
       </c>
       <c r="I17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="9">
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="9">
+        <v>60</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="18" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="D19" s="18">
         <v>0</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H19" s="18">
         <v>0</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="18" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1172,22 +1199,22 @@
         <v>0</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H20" s="18">
         <v>30</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1195,71 +1222,71 @@
         <v>6</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="18">
         <v>10</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H21" s="18">
         <v>60</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="18">
         <v>40</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="20" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="20">
         <v>0</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H23" s="20">
         <v>0</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="20" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1270,19 +1297,19 @@
         <v>0</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H24" s="20">
         <v>70</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -1290,102 +1317,102 @@
         <v>7</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D25" s="20">
         <v>40</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D26" s="20">
         <v>80</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" t="s">
-        <v>24</v>
-      </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" t="s">
         <v>32</v>
-      </c>
-      <c r="F37" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>